<commit_message>
Fixed bug where it would write one cell ahead
</commit_message>
<xml_diff>
--- a/bin/Database/UserInformation/banana.xlsx
+++ b/bin/Database/UserInformation/banana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\UserInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F357FC2-8EA5-414F-AC4B-D05ACD20725C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D788EFB-B907-4F72-9F0B-EE698D96ED44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="3015" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
+    <workbookView xWindow="4980" yWindow="4080" windowWidth="21600" windowHeight="11835" activeTab="4" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Amount" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +416,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>10000</v>
+        <v>10001</v>
       </c>
     </row>
   </sheetData>
@@ -426,13 +426,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -449,6 +451,9 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -456,15 +461,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -481,6 +486,9 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -490,7 +498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2DBD7-70F4-41FB-80F6-FD3DA71A2055}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -517,7 +527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Made excel write function work for all accounts
</commit_message>
<xml_diff>
--- a/bin/Database/UserInformation/banana.xlsx
+++ b/bin/Database/UserInformation/banana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\UserInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D788EFB-B907-4F72-9F0B-EE698D96ED44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833F204F-05B0-4EF2-867F-A4713CDE83D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="4080" windowWidth="21600" windowHeight="11835" activeTab="4" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
+    <workbookView xWindow="4980" yWindow="4080" windowWidth="21600" windowHeight="11835" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Amount" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03CE7BD-B2D0-4A23-9F6B-DC8026FC762A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +454,15 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2"/>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,10 +470,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +498,15 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2"/>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -499,7 +517,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed weird space bug
</commit_message>
<xml_diff>
--- a/bin/Database/UserInformation/banana.xlsx
+++ b/bin/Database/UserInformation/banana.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\UserInformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\User_Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833F204F-05B0-4EF2-867F-A4713CDE83D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B1D8A-DD05-453F-8B59-3EB1347FE1C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="4080" windowWidth="21600" windowHeight="11835" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
+    <workbookView xWindow="5985" yWindow="4305" windowWidth="21600" windowHeight="11835" activeTab="4" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Amount" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Amount</t>
   </si>
@@ -56,12 +56,25 @@
   </si>
   <si>
     <t>Location/Place/Person</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>0900</t>
+  </si>
+  <si>
+    <t>12/06/2021</t>
+  </si>
+  <si>
+    <t>Banana, Porch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,9 +104,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,115 +422,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03CE7BD-B2D0-4A23-9F6B-DC8026FC762A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>10001</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2DBD7-70F4-41FB-80F6-FD3DA71A2055}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -533,7 +449,21 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -541,13 +471,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
-  <dimension ref="A1:D1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -562,6 +490,74 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2DBD7-70F4-41FB-80F6-FD3DA71A2055}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dont worry about it
</commit_message>
<xml_diff>
--- a/bin/Database/UserInformation/banana.xlsx
+++ b/bin/Database/UserInformation/banana.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\User_Information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\UserInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B1D8A-DD05-453F-8B59-3EB1347FE1C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94692313-45FC-4757-AD9E-8AF0C1253988}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="4305" windowWidth="21600" windowHeight="11835" activeTab="4" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
+    <workbookView xWindow="6000" yWindow="3450" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Amount" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>Amount</t>
   </si>
@@ -74,13 +74,15 @@
   </si>
   <si>
     <t>lakeland, port</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,13 +440,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +461,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -472,7 +479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -493,13 +500,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,8 +521,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -527,7 +539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -548,13 +560,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2DBD7-70F4-41FB-80F6-FD3DA71A2055}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,6 +580,9 @@
       </c>
       <c r="D1" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -575,13 +592,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,6 +612,9 @@
       </c>
       <c r="D1" t="s">
         <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Mathew's UI Update to look much better
</commit_message>
<xml_diff>
--- a/bin/Database/UserInformation/banana.xlsx
+++ b/bin/Database/UserInformation/banana.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Amount</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t>Fully small test</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>test, test test</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>2359</t>
+  </si>
+  <si>
+    <t>Omega test</t>
+  </si>
+  <si>
+    <t>No test :(</t>
   </si>
 </sst>
 </file>
@@ -501,7 +522,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -605,6 +626,23 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -612,7 +650,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -714,6 +752,23 @@
       </c>
       <c r="E6" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Exception handling for TextFields
</commit_message>
<xml_diff>
--- a/bin/Database/UserInformation/banana.xlsx
+++ b/bin/Database/UserInformation/banana.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>Amount</t>
   </si>
@@ -537,7 +537,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -673,6 +673,23 @@
       </c>
       <c r="E8" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>